<commit_message>
changed the reference entitiy names in the test dataset as well as in the MappingServiceTest
</commit_message>
<xml_diff>
--- a/src/test/resources/org/molgenis/selenium/mappingservice/mappingservice-test.xlsx
+++ b/src/test/resources/org/molgenis/selenium/mappingservice/mappingservice-test.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14500" tabRatio="500" firstSheet="5" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="18100" tabRatio="500" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="entities" sheetId="1" r:id="rId1"/>
     <sheet name="attributes" sheetId="2" r:id="rId2"/>
-    <sheet name="GENDER_Ref_test" sheetId="3" r:id="rId3"/>
-    <sheet name="NUCHTER1_Ref_test" sheetId="4" r:id="rId4"/>
-    <sheet name="SEX_Ref_test" sheetId="6" r:id="rId5"/>
+    <sheet name="test_GENDER_Ref_test" sheetId="3" r:id="rId3"/>
+    <sheet name="test_NUCHTER1_Ref_test" sheetId="4" r:id="rId4"/>
+    <sheet name="test_SEX_Ref_test" sheetId="6" r:id="rId5"/>
     <sheet name="HOP_GENDER_Ref_selenium" sheetId="10" r:id="rId6"/>
     <sheet name="lifelines_test" sheetId="5" r:id="rId7"/>
     <sheet name="prevend_test" sheetId="7" r:id="rId8"/>
@@ -178,18 +178,9 @@
     <t>lifelines_test</t>
   </si>
   <si>
-    <t>GENDER_Ref_test</t>
-  </si>
-  <si>
-    <t>NUCHTER1_Ref_test</t>
-  </si>
-  <si>
     <t>prevend_test</t>
   </si>
   <si>
-    <t>SEX_Ref_test</t>
-  </si>
-  <si>
     <t>SEX</t>
   </si>
   <si>
@@ -287,6 +278,15 @@
   </si>
   <si>
     <t>Missing</t>
+  </si>
+  <si>
+    <t>test_GENDER_Ref_test</t>
+  </si>
+  <si>
+    <t>test_NUCHTER1_Ref_test</t>
+  </si>
+  <si>
+    <t>test_SEX_Ref_test</t>
   </si>
 </sst>
 </file>
@@ -342,8 +342,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -369,7 +375,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="21">
+  <cellStyles count="27">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -380,6 +386,9 @@
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -390,6 +399,9 @@
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -722,7 +734,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A9:XFD10"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -751,32 +763,32 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -795,7 +807,7 @@
   <dimension ref="A1:S33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -896,7 +908,7 @@
         <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>84</v>
       </c>
       <c r="C3" t="s">
         <v>25</v>
@@ -919,7 +931,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>84</v>
       </c>
       <c r="C4" t="s">
         <v>20</v>
@@ -945,7 +957,7 @@
         <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>85</v>
       </c>
       <c r="C5" t="s">
         <v>25</v>
@@ -968,7 +980,7 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>85</v>
       </c>
       <c r="C6" t="s">
         <v>20</v>
@@ -1003,7 +1015,7 @@
         <v>28</v>
       </c>
       <c r="E7" t="s">
-        <v>50</v>
+        <v>84</v>
       </c>
       <c r="F7" t="s">
         <v>22</v>
@@ -1066,7 +1078,7 @@
         <v>48</v>
       </c>
       <c r="E10" t="s">
-        <v>51</v>
+        <v>85</v>
       </c>
       <c r="F10" t="s">
         <v>22</v>
@@ -1120,7 +1132,7 @@
         <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C13" t="s">
         <v>20</v>
@@ -1146,7 +1158,7 @@
         <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>53</v>
+        <v>86</v>
       </c>
       <c r="C14" t="s">
         <v>25</v>
@@ -1169,7 +1181,7 @@
         <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>53</v>
+        <v>86</v>
       </c>
       <c r="C15" t="s">
         <v>20</v>
@@ -1192,19 +1204,19 @@
     </row>
     <row r="16" spans="1:19">
       <c r="A16" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B16" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C16" t="s">
         <v>27</v>
       </c>
       <c r="D16" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E16" t="s">
-        <v>53</v>
+        <v>86</v>
       </c>
       <c r="F16" t="s">
         <v>22</v>
@@ -1215,16 +1227,16 @@
     </row>
     <row r="17" spans="1:15">
       <c r="A17" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B17" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C17" t="s">
         <v>30</v>
       </c>
       <c r="D17" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F17" t="s">
         <v>22</v>
@@ -1235,16 +1247,16 @@
     </row>
     <row r="18" spans="1:15">
       <c r="A18" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B18" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C18" t="s">
         <v>30</v>
       </c>
       <c r="D18" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F18" t="s">
         <v>22</v>
@@ -1255,16 +1267,16 @@
     </row>
     <row r="19" spans="1:15">
       <c r="A19" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B19" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C19" t="s">
         <v>30</v>
       </c>
       <c r="D19" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F19" t="s">
         <v>22</v>
@@ -1275,16 +1287,16 @@
     </row>
     <row r="20" spans="1:15">
       <c r="A20" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B20" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C20" t="s">
         <v>30</v>
       </c>
       <c r="D20" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F20" t="s">
         <v>22</v>
@@ -1298,7 +1310,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C21" t="s">
         <v>20</v>
@@ -1324,7 +1336,7 @@
         <v>24</v>
       </c>
       <c r="B22" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C22" t="s">
         <v>25</v>
@@ -1347,7 +1359,7 @@
         <v>3</v>
       </c>
       <c r="B23" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C23" t="s">
         <v>20</v>
@@ -1370,19 +1382,19 @@
     </row>
     <row r="24" spans="1:15">
       <c r="A24" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C24" t="s">
         <v>27</v>
       </c>
       <c r="D24" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E24" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F24" t="s">
         <v>22</v>
@@ -1393,16 +1405,16 @@
     </row>
     <row r="25" spans="1:15">
       <c r="A25" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C25" t="s">
         <v>30</v>
       </c>
       <c r="D25" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F25" t="s">
         <v>22</v>
@@ -1413,16 +1425,16 @@
     </row>
     <row r="26" spans="1:15">
       <c r="A26" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C26" t="s">
         <v>30</v>
       </c>
       <c r="D26" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F26" t="s">
         <v>22</v>
@@ -1433,16 +1445,16 @@
     </row>
     <row r="27" spans="1:15">
       <c r="A27" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C27" t="s">
         <v>30</v>
       </c>
       <c r="D27" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F27" t="s">
         <v>22</v>
@@ -1453,16 +1465,16 @@
     </row>
     <row r="28" spans="1:15">
       <c r="A28" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C28" t="s">
         <v>30</v>
       </c>
       <c r="D28" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F28" t="s">
         <v>22</v>
@@ -1473,16 +1485,16 @@
     </row>
     <row r="29" spans="1:15">
       <c r="A29" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C29" t="s">
         <v>30</v>
       </c>
       <c r="D29" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F29" t="s">
         <v>22</v>
@@ -1493,10 +1505,10 @@
     </row>
     <row r="30" spans="1:15">
       <c r="A30" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C30" t="s">
         <v>30</v>
@@ -1513,16 +1525,16 @@
     </row>
     <row r="31" spans="1:15">
       <c r="A31" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C31" t="s">
         <v>30</v>
       </c>
       <c r="D31" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F31" t="s">
         <v>22</v>
@@ -1533,16 +1545,16 @@
     </row>
     <row r="32" spans="1:15">
       <c r="A32" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C32" t="s">
         <v>30</v>
       </c>
       <c r="D32" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F32" t="s">
         <v>22</v>
@@ -1553,16 +1565,16 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C33" t="s">
         <v>30</v>
       </c>
       <c r="D33" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F33" t="s">
         <v>22</v>
@@ -1690,7 +1702,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
         <v>42</v>
@@ -1734,7 +1746,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
         <v>42</v>
@@ -1750,10 +1762,10 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1852,19 +1864,19 @@
         <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:6">

</xml_diff>

<commit_message>
added a new mapping service test for testing advanced funcationalities
</commit_message>
<xml_diff>
--- a/src/test/resources/org/molgenis/selenium/mappingservice/mappingservice-test.xlsx
+++ b/src/test/resources/org/molgenis/selenium/mappingservice/mappingservice-test.xlsx
@@ -4,17 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="18100" tabRatio="500" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="18100" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="entities" sheetId="1" r:id="rId1"/>
     <sheet name="attributes" sheetId="2" r:id="rId2"/>
     <sheet name="test_GENDER_Ref_test" sheetId="3" r:id="rId3"/>
     <sheet name="test_NUCHTER1_Ref_test" sheetId="4" r:id="rId4"/>
-    <sheet name="test_SEX_Ref_test" sheetId="6" r:id="rId5"/>
-    <sheet name="HOP_GENDER_Ref_selenium" sheetId="10" r:id="rId6"/>
-    <sheet name="lifelines_test" sheetId="5" r:id="rId7"/>
-    <sheet name="prevend_test" sheetId="7" r:id="rId8"/>
+    <sheet name="test_FOOD59A1_Ref_test" sheetId="12" r:id="rId5"/>
+    <sheet name="test_SEX_Ref_test" sheetId="6" r:id="rId6"/>
+    <sheet name="HOP_GENDER_Ref_selenium" sheetId="10" r:id="rId7"/>
+    <sheet name="FOOD_POTATOES_Ref_selenium" sheetId="11" r:id="rId8"/>
+    <sheet name="lifelines_test" sheetId="5" r:id="rId9"/>
+    <sheet name="prevend_test" sheetId="7" r:id="rId10"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="109">
   <si>
     <t>name</t>
   </si>
@@ -287,6 +289,72 @@
   </si>
   <si>
     <t>test_SEX_Ref_test</t>
+  </si>
+  <si>
+    <t>FOOD_POTATOES_Ref_selenium</t>
+  </si>
+  <si>
+    <t>Current Consumption Frequency of Potatoes</t>
+  </si>
+  <si>
+    <t>FOOD_POTATOES</t>
+  </si>
+  <si>
+    <t>Almost daily + daily</t>
+  </si>
+  <si>
+    <t>Several times a week</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>About once a week</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Never + fewer than once a week</t>
+  </si>
+  <si>
+    <t>FOOD59A1</t>
+  </si>
+  <si>
+    <t>How often did you eat boiled or mashed potatoes (also in stew) in the past month? Baked potatoes are asked later</t>
+  </si>
+  <si>
+    <t>test_FOOD59A1_Ref_test</t>
+  </si>
+  <si>
+    <t>This month's</t>
+  </si>
+  <si>
+    <t>1 day per month</t>
+  </si>
+  <si>
+    <t>2-3 days per month</t>
+  </si>
+  <si>
+    <t>1 day per week</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>2-3 days per week</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>4-5 days per week</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>6-7 days per week</t>
   </si>
 </sst>
 </file>
@@ -342,8 +410,36 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="27">
+  <cellStyleXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -375,7 +471,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="27">
+  <cellStyles count="55">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -389,6 +485,20 @@
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -402,6 +512,20 @@
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -731,10 +855,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -762,32 +886,37 @@
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>84</v>
+      <c r="A3" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>86</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
         <v>63</v>
       </c>
     </row>
@@ -802,12 +931,132 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>4.5</v>
+      </c>
+      <c r="D2">
+        <v>1.27</v>
+      </c>
+      <c r="E2">
+        <v>160</v>
+      </c>
+      <c r="F2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D3">
+        <v>0.9</v>
+      </c>
+      <c r="E3">
+        <v>177</v>
+      </c>
+      <c r="F3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>4.7</v>
+      </c>
+      <c r="D4">
+        <v>0.53</v>
+      </c>
+      <c r="E4">
+        <v>170</v>
+      </c>
+      <c r="F4">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>4.7</v>
+      </c>
+      <c r="D5">
+        <v>1.31</v>
+      </c>
+      <c r="E5">
+        <v>173</v>
+      </c>
+      <c r="F5">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S33"/>
+  <dimension ref="A1:S39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1003,59 +1252,68 @@
     </row>
     <row r="7" spans="1:19">
       <c r="A7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" t="s">
-        <v>49</v>
+        <v>24</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>98</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" t="s">
-        <v>84</v>
+        <v>24</v>
       </c>
       <c r="F7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G7" t="s">
+        <v>22</v>
+      </c>
+      <c r="K7" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:19">
       <c r="A8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" t="s">
-        <v>49</v>
+        <v>3</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>98</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="F8" t="s">
         <v>22</v>
       </c>
       <c r="G8" t="s">
+        <v>22</v>
+      </c>
+      <c r="K8" t="s">
+        <v>23</v>
+      </c>
+      <c r="L8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:19">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
         <v>49</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>28</v>
+      </c>
+      <c r="E9" t="s">
+        <v>84</v>
       </c>
       <c r="F9" t="s">
         <v>22</v>
@@ -1066,19 +1324,16 @@
     </row>
     <row r="10" spans="1:19">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
         <v>49</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E10" t="s">
-        <v>85</v>
+        <v>31</v>
       </c>
       <c r="F10" t="s">
         <v>22</v>
@@ -1089,7 +1344,7 @@
     </row>
     <row r="11" spans="1:19">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B11" t="s">
         <v>49</v>
@@ -1098,7 +1353,7 @@
         <v>30</v>
       </c>
       <c r="D11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F11" t="s">
         <v>22</v>
@@ -1109,16 +1364,19 @@
     </row>
     <row r="12" spans="1:19">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="B12" t="s">
         <v>49</v>
       </c>
       <c r="C12" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D12" t="s">
-        <v>37</v>
+        <v>48</v>
+      </c>
+      <c r="E12" t="s">
+        <v>85</v>
       </c>
       <c r="F12" t="s">
         <v>22</v>
@@ -1129,154 +1387,157 @@
     </row>
     <row r="13" spans="1:19">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="B13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>30</v>
+      </c>
+      <c r="D13" t="s">
+        <v>35</v>
       </c>
       <c r="F13" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G13" t="s">
-        <v>22</v>
-      </c>
-      <c r="K13" t="s">
-        <v>23</v>
-      </c>
-      <c r="L13" t="s">
-        <v>23</v>
-      </c>
-      <c r="O13" t="b">
-        <v>0</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:19">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="B14" t="s">
-        <v>86</v>
+        <v>49</v>
       </c>
       <c r="C14" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D14" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="F14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G14" t="s">
-        <v>22</v>
-      </c>
-      <c r="K14" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:19">
       <c r="A15" t="s">
-        <v>3</v>
+        <v>96</v>
       </c>
       <c r="B15" t="s">
-        <v>86</v>
+        <v>49</v>
       </c>
       <c r="C15" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D15" t="s">
-        <v>3</v>
+        <v>97</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>98</v>
       </c>
       <c r="F15" t="s">
         <v>22</v>
       </c>
       <c r="G15" t="s">
-        <v>22</v>
-      </c>
-      <c r="K15" t="s">
-        <v>23</v>
-      </c>
-      <c r="L15" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:19">
       <c r="A16" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="B16" t="s">
         <v>50</v>
       </c>
       <c r="C16" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" t="s">
-        <v>52</v>
-      </c>
-      <c r="E16" t="s">
-        <v>86</v>
+        <v>20</v>
       </c>
       <c r="F16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G16" t="s">
-        <v>23</v>
+        <v>22</v>
+      </c>
+      <c r="K16" t="s">
+        <v>23</v>
+      </c>
+      <c r="L16" t="s">
+        <v>23</v>
+      </c>
+      <c r="O16" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:15">
       <c r="A17" t="s">
-        <v>53</v>
+        <v>24</v>
       </c>
       <c r="B17" t="s">
-        <v>50</v>
+        <v>86</v>
       </c>
       <c r="C17" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D17" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="F17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G17" t="s">
+        <v>22</v>
+      </c>
+      <c r="K17" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:15">
       <c r="A18" t="s">
-        <v>55</v>
+        <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>50</v>
+        <v>86</v>
       </c>
       <c r="C18" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D18" t="s">
-        <v>56</v>
+        <v>3</v>
       </c>
       <c r="F18" t="s">
         <v>22</v>
       </c>
       <c r="G18" t="s">
+        <v>22</v>
+      </c>
+      <c r="K18" t="s">
+        <v>23</v>
+      </c>
+      <c r="L18" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:15">
       <c r="A19" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B19" t="s">
         <v>50</v>
       </c>
       <c r="C19" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D19" t="s">
-        <v>58</v>
+        <v>52</v>
+      </c>
+      <c r="E19" t="s">
+        <v>86</v>
       </c>
       <c r="F19" t="s">
         <v>22</v>
@@ -1287,7 +1548,7 @@
     </row>
     <row r="20" spans="1:15">
       <c r="A20" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B20" t="s">
         <v>50</v>
@@ -1296,7 +1557,7 @@
         <v>30</v>
       </c>
       <c r="D20" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="F20" t="s">
         <v>22</v>
@@ -1307,194 +1568,203 @@
     </row>
     <row r="21" spans="1:15">
       <c r="A21" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>62</v>
+        <v>55</v>
+      </c>
+      <c r="B21" t="s">
+        <v>50</v>
       </c>
       <c r="C21" t="s">
-        <v>20</v>
+        <v>30</v>
+      </c>
+      <c r="D21" t="s">
+        <v>56</v>
       </c>
       <c r="F21" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G21" t="s">
-        <v>22</v>
-      </c>
-      <c r="K21" t="s">
-        <v>23</v>
-      </c>
-      <c r="L21" t="s">
-        <v>23</v>
-      </c>
-      <c r="O21" t="b">
-        <v>0</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:15">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="B22" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="C22" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D22" t="s">
-        <v>24</v>
+        <v>58</v>
       </c>
       <c r="F22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G22" t="s">
-        <v>22</v>
-      </c>
-      <c r="K22" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:15">
       <c r="A23" t="s">
-        <v>3</v>
+        <v>59</v>
       </c>
       <c r="B23" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="C23" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D23" t="s">
-        <v>3</v>
+        <v>60</v>
       </c>
       <c r="F23" t="s">
         <v>22</v>
       </c>
       <c r="G23" t="s">
-        <v>22</v>
-      </c>
-      <c r="K23" t="s">
-        <v>23</v>
-      </c>
-      <c r="L23" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:15">
       <c r="A24" t="s">
-        <v>64</v>
+        <v>19</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>62</v>
       </c>
       <c r="C24" t="s">
-        <v>27</v>
-      </c>
-      <c r="D24" t="s">
-        <v>52</v>
-      </c>
-      <c r="E24" t="s">
-        <v>63</v>
+        <v>20</v>
       </c>
       <c r="F24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G24" t="s">
-        <v>23</v>
+        <v>22</v>
+      </c>
+      <c r="K24" t="s">
+        <v>23</v>
+      </c>
+      <c r="L24" t="s">
+        <v>23</v>
+      </c>
+      <c r="O24" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:15">
       <c r="A25" t="s">
-        <v>65</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>62</v>
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>63</v>
       </c>
       <c r="C25" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D25" t="s">
-        <v>66</v>
+        <v>24</v>
       </c>
       <c r="F25" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G25" t="s">
+        <v>22</v>
+      </c>
+      <c r="K25" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:15">
       <c r="A26" t="s">
-        <v>67</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>62</v>
+        <v>3</v>
+      </c>
+      <c r="B26" t="s">
+        <v>63</v>
       </c>
       <c r="C26" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D26" t="s">
-        <v>68</v>
+        <v>3</v>
       </c>
       <c r="F26" t="s">
         <v>22</v>
       </c>
       <c r="G26" t="s">
+        <v>22</v>
+      </c>
+      <c r="K26" t="s">
+        <v>23</v>
+      </c>
+      <c r="L26" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:15">
       <c r="A27" t="s">
-        <v>69</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>62</v>
+        <v>24</v>
+      </c>
+      <c r="B27" t="s">
+        <v>87</v>
       </c>
       <c r="C27" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D27" t="s">
-        <v>70</v>
+        <v>24</v>
       </c>
       <c r="F27" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G27" t="s">
+        <v>22</v>
+      </c>
+      <c r="K27" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:15">
       <c r="A28" t="s">
-        <v>71</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>62</v>
+        <v>3</v>
+      </c>
+      <c r="B28" t="s">
+        <v>87</v>
       </c>
       <c r="C28" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D28" t="s">
-        <v>72</v>
+        <v>3</v>
       </c>
       <c r="F28" t="s">
         <v>22</v>
       </c>
       <c r="G28" t="s">
+        <v>22</v>
+      </c>
+      <c r="K28" t="s">
+        <v>23</v>
+      </c>
+      <c r="L28" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="29" spans="1:15">
       <c r="A29" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>62</v>
       </c>
       <c r="C29" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D29" t="s">
-        <v>74</v>
+        <v>52</v>
+      </c>
+      <c r="E29" t="s">
+        <v>63</v>
       </c>
       <c r="F29" t="s">
         <v>22</v>
@@ -1505,7 +1775,7 @@
     </row>
     <row r="30" spans="1:15">
       <c r="A30" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>62</v>
@@ -1514,7 +1784,7 @@
         <v>30</v>
       </c>
       <c r="D30" t="s">
-        <v>37</v>
+        <v>66</v>
       </c>
       <c r="F30" t="s">
         <v>22</v>
@@ -1525,7 +1795,7 @@
     </row>
     <row r="31" spans="1:15">
       <c r="A31" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>62</v>
@@ -1534,7 +1804,7 @@
         <v>30</v>
       </c>
       <c r="D31" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="F31" t="s">
         <v>22</v>
@@ -1545,7 +1815,7 @@
     </row>
     <row r="32" spans="1:15">
       <c r="A32" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>62</v>
@@ -1554,7 +1824,7 @@
         <v>30</v>
       </c>
       <c r="D32" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="F32" t="s">
         <v>22</v>
@@ -1565,7 +1835,7 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>62</v>
@@ -1574,12 +1844,135 @@
         <v>30</v>
       </c>
       <c r="D33" t="s">
+        <v>72</v>
+      </c>
+      <c r="F33" t="s">
+        <v>22</v>
+      </c>
+      <c r="G33" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" t="s">
+        <v>73</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C34" t="s">
+        <v>30</v>
+      </c>
+      <c r="D34" t="s">
+        <v>74</v>
+      </c>
+      <c r="F34" t="s">
+        <v>22</v>
+      </c>
+      <c r="G34" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" t="s">
+        <v>75</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C35" t="s">
+        <v>30</v>
+      </c>
+      <c r="D35" t="s">
+        <v>37</v>
+      </c>
+      <c r="F35" t="s">
+        <v>22</v>
+      </c>
+      <c r="G35" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" t="s">
+        <v>76</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C36" t="s">
+        <v>30</v>
+      </c>
+      <c r="D36" t="s">
+        <v>77</v>
+      </c>
+      <c r="F36" t="s">
+        <v>22</v>
+      </c>
+      <c r="G36" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" t="s">
+        <v>78</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C37" t="s">
+        <v>30</v>
+      </c>
+      <c r="D37" t="s">
+        <v>79</v>
+      </c>
+      <c r="F37" t="s">
+        <v>22</v>
+      </c>
+      <c r="G37" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" t="s">
+        <v>80</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C38" t="s">
+        <v>30</v>
+      </c>
+      <c r="D38" t="s">
         <v>81</v>
       </c>
-      <c r="F33" t="s">
-        <v>22</v>
-      </c>
-      <c r="G33" t="s">
+      <c r="F38" t="s">
+        <v>22</v>
+      </c>
+      <c r="G38" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" t="s">
+        <v>89</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C39" t="s">
+        <v>27</v>
+      </c>
+      <c r="D39" t="s">
+        <v>88</v>
+      </c>
+      <c r="E39" t="s">
+        <v>87</v>
+      </c>
+      <c r="F39" t="s">
+        <v>22</v>
+      </c>
+      <c r="G39" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1684,13 +2077,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="17.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -1702,18 +2098,58 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B8" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1728,6 +2164,50 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1778,7 +2258,78 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="27.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -1847,124 +2398,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2">
-        <v>4</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>4.5</v>
-      </c>
-      <c r="D2">
-        <v>1.27</v>
-      </c>
-      <c r="E2">
-        <v>160</v>
-      </c>
-      <c r="F2">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3">
-        <v>6</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="D3">
-        <v>0.9</v>
-      </c>
-      <c r="E3">
-        <v>177</v>
-      </c>
-      <c r="F3">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>4.7</v>
-      </c>
-      <c r="D4">
-        <v>0.53</v>
-      </c>
-      <c r="E4">
-        <v>170</v>
-      </c>
-      <c r="F4">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>4.7</v>
-      </c>
-      <c r="D5">
-        <v>1.31</v>
-      </c>
-      <c r="E5">
-        <v>173</v>
-      </c>
-      <c r="F5">
-        <v>76</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
added the advanced selenium-test for mapping service
</commit_message>
<xml_diff>
--- a/src/test/resources/org/molgenis/selenium/mappingservice/mappingservice-test.xlsx
+++ b/src/test/resources/org/molgenis/selenium/mappingservice/mappingservice-test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="18100" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="18100" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="entities" sheetId="1" r:id="rId1"/>
@@ -14,9 +14,11 @@
     <sheet name="test_FOOD59A1_Ref_test" sheetId="12" r:id="rId5"/>
     <sheet name="test_SEX_Ref_test" sheetId="6" r:id="rId6"/>
     <sheet name="HOP_GENDER_Ref_selenium" sheetId="10" r:id="rId7"/>
-    <sheet name="FOOD_POTATOES_Ref_selenium" sheetId="11" r:id="rId8"/>
-    <sheet name="lifelines_test" sheetId="5" r:id="rId9"/>
-    <sheet name="prevend_test" sheetId="7" r:id="rId10"/>
+    <sheet name="DIS_HBP_Ref_selenium" sheetId="13" r:id="rId8"/>
+    <sheet name="FOOD_POTATOES_Ref_selenium" sheetId="11" r:id="rId9"/>
+    <sheet name="test_HEALTH351_Ref_test" sheetId="14" r:id="rId10"/>
+    <sheet name="lifelines_test" sheetId="5" r:id="rId11"/>
+    <sheet name="prevend_test" sheetId="7" r:id="rId12"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="118">
   <si>
     <t>name</t>
   </si>
@@ -327,9 +329,6 @@
     <t>test_FOOD59A1_Ref_test</t>
   </si>
   <si>
-    <t>This month's</t>
-  </si>
-  <si>
     <t>1 day per month</t>
   </si>
   <si>
@@ -355,6 +354,36 @@
   </si>
   <si>
     <t>6-7 days per week</t>
+  </si>
+  <si>
+    <t>Not this month</t>
+  </si>
+  <si>
+    <t>HEALTH351</t>
+  </si>
+  <si>
+    <t>Have you ever had high blood pressure? (Repeat) (1)</t>
+  </si>
+  <si>
+    <t>test_HEALTH351_Ref_test</t>
+  </si>
+  <si>
+    <t>I do not know</t>
+  </si>
+  <si>
+    <t>DIS_HBP</t>
+  </si>
+  <si>
+    <t>History of Hypertension</t>
+  </si>
+  <si>
+    <t>DIS_HBP_Ref_selenium</t>
+  </si>
+  <si>
+    <t>Never had high blood pressure</t>
+  </si>
+  <si>
+    <t>Ever had high blood pressure</t>
   </si>
 </sst>
 </file>
@@ -410,8 +439,48 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="55">
+  <cellStyleXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -471,7 +540,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="55">
+  <cellStyles count="95">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -499,6 +568,26 @@
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -526,6 +615,26 @@
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -855,10 +964,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -901,23 +1010,33 @@
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>50</v>
+      <c r="A6" s="1" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>86</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
         <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="1" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -933,6 +1052,141 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="4" max="4" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" t="s">
+        <v>96</v>
+      </c>
+      <c r="I1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2">
+        <v>3498377</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>167.5</v>
+      </c>
+      <c r="D2">
+        <v>98000</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>6.6</v>
+      </c>
+      <c r="G2">
+        <v>1.04</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1053,10 +1307,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S39"/>
+  <dimension ref="A1:S45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1301,59 +1555,68 @@
     </row>
     <row r="9" spans="1:19">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>111</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" t="s">
-        <v>84</v>
+        <v>24</v>
       </c>
       <c r="F9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G9" t="s">
+        <v>22</v>
+      </c>
+      <c r="K9" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:19">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>111</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="F10" t="s">
         <v>22</v>
       </c>
       <c r="G10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K10" t="s">
+        <v>23</v>
+      </c>
+      <c r="L10" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:19">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B11" t="s">
         <v>49</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D11" t="s">
-        <v>33</v>
+        <v>28</v>
+      </c>
+      <c r="E11" t="s">
+        <v>84</v>
       </c>
       <c r="F11" t="s">
         <v>22</v>
@@ -1364,19 +1627,16 @@
     </row>
     <row r="12" spans="1:19">
       <c r="A12" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="B12" t="s">
         <v>49</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D12" t="s">
-        <v>48</v>
-      </c>
-      <c r="E12" t="s">
-        <v>85</v>
+        <v>31</v>
       </c>
       <c r="F12" t="s">
         <v>22</v>
@@ -1387,7 +1647,7 @@
     </row>
     <row r="13" spans="1:19">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B13" t="s">
         <v>49</v>
@@ -1396,7 +1656,7 @@
         <v>30</v>
       </c>
       <c r="D13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F13" t="s">
         <v>22</v>
@@ -1407,16 +1667,19 @@
     </row>
     <row r="14" spans="1:19">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="B14" t="s">
         <v>49</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D14" t="s">
-        <v>37</v>
+        <v>48</v>
+      </c>
+      <c r="E14" t="s">
+        <v>85</v>
       </c>
       <c r="F14" t="s">
         <v>22</v>
@@ -1427,19 +1690,16 @@
     </row>
     <row r="15" spans="1:19">
       <c r="A15" t="s">
-        <v>96</v>
+        <v>34</v>
       </c>
       <c r="B15" t="s">
         <v>49</v>
       </c>
       <c r="C15" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D15" t="s">
-        <v>97</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>98</v>
+        <v>35</v>
       </c>
       <c r="F15" t="s">
         <v>22</v>
@@ -1450,154 +1710,160 @@
     </row>
     <row r="16" spans="1:19">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="B16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C16" t="s">
-        <v>20</v>
+        <v>30</v>
+      </c>
+      <c r="D16" t="s">
+        <v>37</v>
       </c>
       <c r="F16" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G16" t="s">
-        <v>22</v>
-      </c>
-      <c r="K16" t="s">
-        <v>23</v>
-      </c>
-      <c r="L16" t="s">
-        <v>23</v>
-      </c>
-      <c r="O16" t="b">
-        <v>0</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:15">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>96</v>
       </c>
       <c r="B17" t="s">
-        <v>86</v>
+        <v>49</v>
       </c>
       <c r="C17" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D17" t="s">
-        <v>24</v>
+        <v>97</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>98</v>
       </c>
       <c r="F17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G17" t="s">
-        <v>22</v>
-      </c>
-      <c r="K17" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:15">
       <c r="A18" t="s">
-        <v>3</v>
+        <v>109</v>
       </c>
       <c r="B18" t="s">
-        <v>86</v>
+        <v>49</v>
       </c>
       <c r="C18" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D18" t="s">
-        <v>3</v>
+        <v>110</v>
+      </c>
+      <c r="E18" t="s">
+        <v>111</v>
       </c>
       <c r="F18" t="s">
         <v>22</v>
       </c>
       <c r="G18" t="s">
-        <v>22</v>
-      </c>
-      <c r="K18" t="s">
-        <v>23</v>
-      </c>
-      <c r="L18" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:15">
       <c r="A19" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="B19" t="s">
         <v>50</v>
       </c>
       <c r="C19" t="s">
-        <v>27</v>
-      </c>
-      <c r="D19" t="s">
-        <v>52</v>
-      </c>
-      <c r="E19" t="s">
-        <v>86</v>
+        <v>20</v>
       </c>
       <c r="F19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G19" t="s">
-        <v>23</v>
+        <v>22</v>
+      </c>
+      <c r="K19" t="s">
+        <v>23</v>
+      </c>
+      <c r="L19" t="s">
+        <v>23</v>
+      </c>
+      <c r="O19" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:15">
       <c r="A20" t="s">
-        <v>53</v>
+        <v>24</v>
       </c>
       <c r="B20" t="s">
-        <v>50</v>
+        <v>86</v>
       </c>
       <c r="C20" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D20" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="F20" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G20" t="s">
+        <v>22</v>
+      </c>
+      <c r="K20" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:15">
       <c r="A21" t="s">
-        <v>55</v>
+        <v>3</v>
       </c>
       <c r="B21" t="s">
-        <v>50</v>
+        <v>86</v>
       </c>
       <c r="C21" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D21" t="s">
-        <v>56</v>
+        <v>3</v>
       </c>
       <c r="F21" t="s">
         <v>22</v>
       </c>
       <c r="G21" t="s">
+        <v>22</v>
+      </c>
+      <c r="K21" t="s">
+        <v>23</v>
+      </c>
+      <c r="L21" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:15">
       <c r="A22" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B22" t="s">
         <v>50</v>
       </c>
       <c r="C22" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D22" t="s">
-        <v>58</v>
+        <v>52</v>
+      </c>
+      <c r="E22" t="s">
+        <v>86</v>
       </c>
       <c r="F22" t="s">
         <v>22</v>
@@ -1608,7 +1874,7 @@
     </row>
     <row r="23" spans="1:15">
       <c r="A23" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B23" t="s">
         <v>50</v>
@@ -1617,7 +1883,7 @@
         <v>30</v>
       </c>
       <c r="D23" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="F23" t="s">
         <v>22</v>
@@ -1628,243 +1894,252 @@
     </row>
     <row r="24" spans="1:15">
       <c r="A24" t="s">
-        <v>19</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>62</v>
+        <v>55</v>
+      </c>
+      <c r="B24" t="s">
+        <v>50</v>
       </c>
       <c r="C24" t="s">
-        <v>20</v>
+        <v>30</v>
+      </c>
+      <c r="D24" t="s">
+        <v>56</v>
       </c>
       <c r="F24" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G24" t="s">
-        <v>22</v>
-      </c>
-      <c r="K24" t="s">
-        <v>23</v>
-      </c>
-      <c r="L24" t="s">
-        <v>23</v>
-      </c>
-      <c r="O24" t="b">
-        <v>0</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:15">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="B25" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="C25" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D25" t="s">
-        <v>24</v>
+        <v>58</v>
       </c>
       <c r="F25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G25" t="s">
-        <v>22</v>
-      </c>
-      <c r="K25" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:15">
       <c r="A26" t="s">
-        <v>3</v>
+        <v>59</v>
       </c>
       <c r="B26" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="C26" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D26" t="s">
-        <v>3</v>
+        <v>60</v>
       </c>
       <c r="F26" t="s">
         <v>22</v>
       </c>
       <c r="G26" t="s">
-        <v>22</v>
-      </c>
-      <c r="K26" t="s">
-        <v>23</v>
-      </c>
-      <c r="L26" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:15">
       <c r="A27" t="s">
-        <v>24</v>
-      </c>
-      <c r="B27" t="s">
-        <v>87</v>
+        <v>19</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>62</v>
       </c>
       <c r="C27" t="s">
-        <v>25</v>
-      </c>
-      <c r="D27" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F27" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G27" t="s">
         <v>22</v>
       </c>
       <c r="K27" t="s">
         <v>23</v>
+      </c>
+      <c r="L27" t="s">
+        <v>23</v>
+      </c>
+      <c r="O27" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:15">
       <c r="A28" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="B28" t="s">
-        <v>87</v>
+        <v>63</v>
       </c>
       <c r="C28" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D28" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="F28" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G28" t="s">
         <v>22</v>
       </c>
       <c r="K28" t="s">
-        <v>23</v>
-      </c>
-      <c r="L28" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="29" spans="1:15">
       <c r="A29" t="s">
-        <v>64</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>62</v>
+        <v>3</v>
+      </c>
+      <c r="B29" t="s">
+        <v>63</v>
       </c>
       <c r="C29" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D29" t="s">
-        <v>52</v>
-      </c>
-      <c r="E29" t="s">
-        <v>63</v>
+        <v>3</v>
       </c>
       <c r="F29" t="s">
         <v>22</v>
       </c>
       <c r="G29" t="s">
+        <v>22</v>
+      </c>
+      <c r="K29" t="s">
+        <v>23</v>
+      </c>
+      <c r="L29" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="30" spans="1:15">
       <c r="A30" t="s">
-        <v>65</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>62</v>
+        <v>24</v>
+      </c>
+      <c r="B30" t="s">
+        <v>87</v>
       </c>
       <c r="C30" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D30" t="s">
-        <v>66</v>
+        <v>24</v>
       </c>
       <c r="F30" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G30" t="s">
+        <v>22</v>
+      </c>
+      <c r="K30" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:15">
       <c r="A31" t="s">
-        <v>67</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>62</v>
+        <v>3</v>
+      </c>
+      <c r="B31" t="s">
+        <v>87</v>
       </c>
       <c r="C31" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D31" t="s">
-        <v>68</v>
+        <v>3</v>
       </c>
       <c r="F31" t="s">
         <v>22</v>
       </c>
       <c r="G31" t="s">
+        <v>22</v>
+      </c>
+      <c r="K31" t="s">
+        <v>23</v>
+      </c>
+      <c r="L31" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="32" spans="1:15">
       <c r="A32" t="s">
-        <v>69</v>
+        <v>24</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>62</v>
+        <v>115</v>
       </c>
       <c r="C32" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D32" t="s">
-        <v>70</v>
+        <v>24</v>
       </c>
       <c r="F32" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G32" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
+        <v>22</v>
+      </c>
+      <c r="K32" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
       <c r="A33" t="s">
-        <v>71</v>
+        <v>3</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>62</v>
+        <v>115</v>
       </c>
       <c r="C33" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D33" t="s">
-        <v>72</v>
+        <v>3</v>
       </c>
       <c r="F33" t="s">
         <v>22</v>
       </c>
       <c r="G33" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7">
+        <v>22</v>
+      </c>
+      <c r="K33" t="s">
+        <v>23</v>
+      </c>
+      <c r="L33" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12">
       <c r="A34" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>62</v>
       </c>
       <c r="C34" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D34" t="s">
-        <v>74</v>
+        <v>52</v>
+      </c>
+      <c r="E34" t="s">
+        <v>63</v>
       </c>
       <c r="F34" t="s">
         <v>22</v>
@@ -1873,9 +2148,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:12">
       <c r="A35" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>62</v>
@@ -1884,7 +2159,7 @@
         <v>30</v>
       </c>
       <c r="D35" t="s">
-        <v>37</v>
+        <v>66</v>
       </c>
       <c r="F35" t="s">
         <v>22</v>
@@ -1893,9 +2168,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:12">
       <c r="A36" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>62</v>
@@ -1904,7 +2179,7 @@
         <v>30</v>
       </c>
       <c r="D36" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="F36" t="s">
         <v>22</v>
@@ -1913,9 +2188,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:12">
       <c r="A37" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>62</v>
@@ -1924,7 +2199,7 @@
         <v>30</v>
       </c>
       <c r="D37" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="F37" t="s">
         <v>22</v>
@@ -1933,9 +2208,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:12">
       <c r="A38" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>62</v>
@@ -1944,7 +2219,7 @@
         <v>30</v>
       </c>
       <c r="D38" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F38" t="s">
         <v>22</v>
@@ -1953,26 +2228,149 @@
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:12">
       <c r="A39" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>62</v>
       </c>
       <c r="C39" t="s">
+        <v>30</v>
+      </c>
+      <c r="D39" t="s">
+        <v>74</v>
+      </c>
+      <c r="F39" t="s">
+        <v>22</v>
+      </c>
+      <c r="G39" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12">
+      <c r="A40" t="s">
+        <v>75</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C40" t="s">
+        <v>30</v>
+      </c>
+      <c r="D40" t="s">
+        <v>37</v>
+      </c>
+      <c r="F40" t="s">
+        <v>22</v>
+      </c>
+      <c r="G40" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12">
+      <c r="A41" t="s">
+        <v>76</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C41" t="s">
+        <v>30</v>
+      </c>
+      <c r="D41" t="s">
+        <v>77</v>
+      </c>
+      <c r="F41" t="s">
+        <v>22</v>
+      </c>
+      <c r="G41" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12">
+      <c r="A42" t="s">
+        <v>78</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C42" t="s">
+        <v>30</v>
+      </c>
+      <c r="D42" t="s">
+        <v>79</v>
+      </c>
+      <c r="F42" t="s">
+        <v>22</v>
+      </c>
+      <c r="G42" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12">
+      <c r="A43" t="s">
+        <v>80</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C43" t="s">
+        <v>30</v>
+      </c>
+      <c r="D43" t="s">
+        <v>81</v>
+      </c>
+      <c r="F43" t="s">
+        <v>22</v>
+      </c>
+      <c r="G43" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12">
+      <c r="A44" t="s">
+        <v>89</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C44" t="s">
         <v>27</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D44" t="s">
         <v>88</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E44" t="s">
         <v>87</v>
       </c>
-      <c r="F39" t="s">
-        <v>22</v>
-      </c>
-      <c r="G39" t="s">
+      <c r="F44" t="s">
+        <v>22</v>
+      </c>
+      <c r="G44" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12">
+      <c r="A45" t="s">
+        <v>113</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C45" t="s">
+        <v>27</v>
+      </c>
+      <c r="D45" t="s">
+        <v>114</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F45" t="s">
+        <v>22</v>
+      </c>
+      <c r="G45" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2079,7 +2477,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -2101,7 +2499,7 @@
         <v>41</v>
       </c>
       <c r="B2" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2109,7 +2507,7 @@
         <v>43</v>
       </c>
       <c r="B3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2117,7 +2515,7 @@
         <v>92</v>
       </c>
       <c r="B4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2125,31 +2523,31 @@
         <v>94</v>
       </c>
       <c r="B5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B6" t="s">
         <v>103</v>
-      </c>
-      <c r="B6" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
+        <v>104</v>
+      </c>
+      <c r="B7" t="s">
         <v>105</v>
-      </c>
-      <c r="B7" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
+        <v>106</v>
+      </c>
+      <c r="B8" t="s">
         <v>107</v>
-      </c>
-      <c r="B8" t="s">
-        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -2260,6 +2658,58 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="A1:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2327,75 +2777,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="4" max="4" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2">
-        <v>3498377</v>
-      </c>
-      <c r="B2">
-        <v>2</v>
-      </c>
-      <c r="C2">
-        <v>167.5</v>
-      </c>
-      <c r="D2">
-        <v>98000</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>6.6</v>
-      </c>
-      <c r="G2">
-        <v>1.04</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>